<commit_message>
Improved Phased array data tranmission range
</commit_message>
<xml_diff>
--- a/GameData/WarpPlugin/Parts/BeamedPower/BeamedPower.xlsx
+++ b/GameData/WarpPlugin/Parts/BeamedPower/BeamedPower.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\KSP-Interstellar-Extended\GameData\WarpPlugin\Parts\BeamedPower\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A638C3-7AE7-47AD-901F-52E5FFEDA33E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18615" windowHeight="11370"/>
+    <workbookView xWindow="-60945" yWindow="-1275" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
   <si>
     <t>Transmit</t>
   </si>
@@ -76,12 +82,24 @@
   </si>
   <si>
     <t>Multi Bandwidth Dish Transceiver (shielded)</t>
+  </si>
+  <si>
+    <t>RELAY</t>
+  </si>
+  <si>
+    <t>1.0e+11</t>
+  </si>
+  <si>
+    <t>2.0e+11</t>
+  </si>
+  <si>
+    <t>1.0e+12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,18 +437,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,12 +456,12 @@
     <col min="1" max="3" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -463,7 +481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -488,8 +506,14 @@
       <c r="H3">
         <v>6000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -509,13 +533,19 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>3000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -540,8 +570,14 @@
       <c r="H5">
         <v>1500</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -566,8 +602,14 @@
       <c r="H6">
         <v>1500</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -592,8 +634,14 @@
       <c r="H7">
         <v>900</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -619,7 +667,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -636,7 +684,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -653,7 +701,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>

</xml_diff>